<commit_message>
new fine litter fall code
</commit_message>
<xml_diff>
--- a/Total_soil_respiration/respiration_soil_total meta_data.xlsx
+++ b/Total_soil_respiration/respiration_soil_total meta_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Side_project\african_data_workshop\gem_code_examples\Total_soil_respiration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DF92790-9F98-40C3-BD7C-245853E3802B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D204C285-D073-4399-B43B-58C3B209A38F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-168" yWindow="-19380" windowWidth="25332" windowHeight="17616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="respiration_soil_total meta_dat" sheetId="1" r:id="rId1"/>
@@ -64,15 +64,9 @@
     <t>co2ref</t>
   </si>
   <si>
-    <t>input_d</t>
-  </si>
-  <si>
     <t>time</t>
   </si>
   <si>
-    <t>input_f</t>
-  </si>
-  <si>
     <t>atmp</t>
   </si>
   <si>
@@ -113,6 +107,12 @@
   </si>
   <si>
     <t>see column D, should be relative change in co2 ppm</t>
+  </si>
+  <si>
+    <t>InputD</t>
+  </si>
+  <si>
+    <t>InputF</t>
   </si>
 </sst>
 </file>
@@ -1008,7 +1008,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1045,7 +1045,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1073,7 +1073,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1091,65 +1091,65 @@
         <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>